<commit_message>
Changes added after first peer-review round. Turnaround time and parameter a adjusted
</commit_message>
<xml_diff>
--- a/Text_files/data/Sensitivity_fit.xlsx
+++ b/Text_files/data/Sensitivity_fit.xlsx
@@ -432,19 +432,19 @@
         <v>0.00296318905128447</v>
       </c>
       <c r="D2">
-        <v>0.0003300681264637086</v>
+        <v>-0.002197727961364223</v>
       </c>
       <c r="E2">
-        <v>0.005596309976105232</v>
+        <v>0.008124106063933163</v>
       </c>
       <c r="F2">
         <v>0.0001180266354911932</v>
       </c>
       <c r="G2">
-        <v>3.985549343586825E-05</v>
+        <v>-3.51888029372437E-05</v>
       </c>
       <c r="H2">
-        <v>0.0001961977775465181</v>
+        <v>0.0002712420739196301</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -458,19 +458,19 @@
         <v>0.0138451245522685</v>
       </c>
       <c r="D3">
-        <v>0.00452566667153901</v>
+        <v>-0.004421012893961299</v>
       </c>
       <c r="E3">
-        <v>0.02316458243299799</v>
+        <v>0.0321112619984983</v>
       </c>
       <c r="F3">
         <v>0.0006899026690724931</v>
       </c>
       <c r="G3">
-        <v>0.0003208903245415832</v>
+        <v>-3.336152620809021E-05</v>
       </c>
       <c r="H3">
-        <v>0.001058915013603403</v>
+        <v>0.001413166864353077</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -484,19 +484,19 @@
         <v>0.03364576443777532</v>
       </c>
       <c r="D4">
-        <v>0.01504224893184357</v>
+        <v>-0.002817125953850905</v>
       </c>
       <c r="E4">
-        <v>0.05224927994370707</v>
+        <v>0.07010865482940154</v>
       </c>
       <c r="F4">
         <v>0.001936176800619075</v>
       </c>
       <c r="G4">
-        <v>0.001025146348341401</v>
+        <v>0.0001505571141548338</v>
       </c>
       <c r="H4">
-        <v>0.00284720725289675</v>
+        <v>0.003721796487083317</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -510,19 +510,19 @@
         <v>0.062196663504356</v>
       </c>
       <c r="D5">
-        <v>0.03285273622625784</v>
+        <v>0.004682566039283603</v>
       </c>
       <c r="E5">
-        <v>0.09154059078245416</v>
+        <v>0.1197107609694284</v>
       </c>
       <c r="F5">
         <v>0.004021552577310984</v>
       </c>
       <c r="G5">
-        <v>0.002285728946198403</v>
+        <v>0.000619338260330326</v>
       </c>
       <c r="H5">
-        <v>0.005757376208423565</v>
+        <v>0.007423766894291643</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -536,19 +536,19 @@
         <v>0.09855359895019064</v>
       </c>
       <c r="D6">
-        <v>0.0579210105416981</v>
+        <v>0.01891372566954527</v>
       </c>
       <c r="E6">
-        <v>0.1391861873586832</v>
+        <v>0.178193472230836</v>
       </c>
       <c r="F6">
         <v>0.007079381236473285</v>
       </c>
       <c r="G6">
-        <v>0.004202941100474606</v>
+        <v>0.001441558569915874</v>
       </c>
       <c r="H6">
-        <v>0.009955821372471965</v>
+        <v>0.0127172039030307</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -562,19 +562,19 @@
         <v>0.1412432725047284</v>
       </c>
       <c r="D7">
-        <v>0.08946937640150063</v>
+        <v>0.03976643614240201</v>
       </c>
       <c r="E7">
-        <v>0.1930171686079561</v>
+        <v>0.2427201088670548</v>
       </c>
       <c r="F7">
         <v>0.01121871708076507</v>
       </c>
       <c r="G7">
-        <v>0.00685228582986928</v>
+        <v>0.00266051182900932</v>
       </c>
       <c r="H7">
-        <v>0.01558514833166086</v>
+        <v>0.01977692233252082</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -588,19 +588,19 @@
         <v>0.1885122551394636</v>
       </c>
       <c r="D8">
-        <v>0.126255676052961</v>
+        <v>0.0664893601299186</v>
       </c>
       <c r="E8">
-        <v>0.2507688342259661</v>
+        <v>0.3105351501490086</v>
       </c>
       <c r="F8">
         <v>0.01652695780371907</v>
       </c>
       <c r="G8">
-        <v>0.01028971738183966</v>
+        <v>0.004301966576835427</v>
       </c>
       <c r="H8">
-        <v>0.02276419822559848</v>
+        <v>0.02875194903060271</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -614,19 +614,19 @@
         <v>0.2385587239638908</v>
       </c>
       <c r="D9">
-        <v>0.1668384177117939</v>
+        <v>0.09798692370978074</v>
       </c>
       <c r="E9">
-        <v>0.3102790302159878</v>
+        <v>0.3791305242180009</v>
       </c>
       <c r="F9">
         <v>0.02307082635057682</v>
       </c>
       <c r="G9">
-        <v>0.01455546211252394</v>
+        <v>0.006380712443993186</v>
       </c>
       <c r="H9">
-        <v>0.03158619058862969</v>
+        <v>0.03976094025716045</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -640,19 +640,19 @@
         <v>0.2897157511890584</v>
       </c>
       <c r="D10">
-        <v>0.2097876269900198</v>
+        <v>0.1330566277589428</v>
       </c>
       <c r="E10">
-        <v>0.369643875388097</v>
+        <v>0.446374874619174</v>
       </c>
       <c r="F10">
         <v>0.03089670579799535</v>
       </c>
       <c r="G10">
-        <v>0.01967689735779623</v>
+        <v>0.00890588125520508</v>
       </c>
       <c r="H10">
-        <v>0.04211651423819446</v>
+        <v>0.05288753034078561</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -666,19 +666,19 @@
         <v>0.3405692058425684</v>
       </c>
       <c r="D11">
-        <v>0.2538215156698398</v>
+        <v>0.1705437331040203</v>
       </c>
       <c r="E11">
-        <v>0.4273168960152971</v>
+        <v>0.5105946785811166</v>
       </c>
       <c r="F11">
         <v>0.04003080548255282</v>
       </c>
       <c r="G11">
-        <v>0.02567073636190496</v>
+        <v>0.01188507000608301</v>
       </c>
       <c r="H11">
-        <v>0.05439087460320068</v>
+        <v>0.06817654095902263</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -692,19 +692,19 @@
         <v>0.3900112285809134</v>
       </c>
       <c r="D12">
-        <v>0.2978741921332534</v>
+        <v>0.2094226371434998</v>
       </c>
       <c r="E12">
-        <v>0.4821482650285733</v>
+        <v>0.5705998200183269</v>
       </c>
       <c r="F12">
         <v>0.05047941964415572</v>
       </c>
       <c r="G12">
-        <v>0.03254467884683138</v>
+        <v>0.01532732768140001</v>
       </c>
       <c r="H12">
-        <v>0.06841416044148006</v>
+        <v>0.08563151160691143</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -718,19 +718,19 @@
         <v>0.437242565330151</v>
       </c>
       <c r="D13">
-        <v>0.3411127732229693</v>
+        <v>0.2488281728000749</v>
       </c>
       <c r="E13">
-        <v>0.5333723574373328</v>
+        <v>0.6256569578602271</v>
       </c>
       <c r="F13">
         <v>0.06222942948459545</v>
       </c>
       <c r="G13">
-        <v>0.04029864304778419</v>
+        <v>0.01924508806844537</v>
       </c>
       <c r="H13">
-        <v>0.08416021592140671</v>
+        <v>0.1052137709007455</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -744,19 +744,19 @@
         <v>0.4817416528910525</v>
       </c>
       <c r="D14">
-        <v>0.382923758625847</v>
+        <v>0.2880585801312497</v>
       </c>
       <c r="E14">
-        <v>0.5805595471562579</v>
+        <v>0.6754247256508552</v>
       </c>
       <c r="F14">
         <v>0.07524913128740685</v>
       </c>
       <c r="G14">
-        <v>0.04892566834328825</v>
+        <v>0.02365514391693439</v>
       </c>
       <c r="H14">
-        <v>0.1015725942315254</v>
+        <v>0.1268431186578793</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -770,19 +770,19 @@
         <v>0.5232170646098429</v>
       </c>
       <c r="D15">
-        <v>0.4228841871322448</v>
+        <v>0.3265646247537508</v>
       </c>
       <c r="E15">
-        <v>0.6235499420874409</v>
+        <v>0.7198695044659349</v>
       </c>
       <c r="F15">
         <v>0.08948942421070201</v>
       </c>
       <c r="G15">
-        <v>0.05841256076645726</v>
+        <v>0.0285787718599823</v>
       </c>
       <c r="H15">
-        <v>0.1205662876549468</v>
+        <v>0.1504000765614217</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -796,19 +796,19 @@
         <v>0.5615557259447052</v>
       </c>
       <c r="D16">
-        <v>0.4607276770992804</v>
+        <v>0.3639327502076726</v>
       </c>
       <c r="E16">
-        <v>0.66238377479013</v>
+        <v>0.7591787016817377</v>
       </c>
       <c r="F16">
         <v>0.1048853530507326</v>
       </c>
       <c r="G16">
-        <v>0.06874034382893357</v>
+        <v>0.03404113497600648</v>
       </c>
       <c r="H16">
-        <v>0.1410303622725317</v>
+        <v>0.1757295711254588</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -822,19 +822,19 @@
         <v>0.5967746068546358</v>
       </c>
       <c r="D17">
-        <v>0.4963111060727216</v>
+        <v>0.399866145322084</v>
       </c>
       <c r="E17">
-        <v>0.69723810763655</v>
+        <v>0.7936830683871876</v>
       </c>
       <c r="F17">
         <v>0.1213579707630146</v>
       </c>
       <c r="G17">
-        <v>0.07988457174105992</v>
+        <v>0.04007010867998347</v>
       </c>
       <c r="H17">
-        <v>0.1628313697849692</v>
+        <v>0.2026458328460457</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -848,19 +848,19 @@
         <v>0.6289797058766261</v>
       </c>
       <c r="D18">
-        <v>0.5295847879795078</v>
+        <v>0.4341656667982742</v>
       </c>
       <c r="E18">
-        <v>0.7283746237737444</v>
+        <v>0.8237937449549779</v>
       </c>
       <c r="F18">
         <v>0.1388164621110504</v>
       </c>
       <c r="G18">
-        <v>0.09181555875954064</v>
+        <v>0.0466946915420913</v>
       </c>
       <c r="H18">
-        <v>0.1858173654625601</v>
+        <v>0.2309382326800094</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -874,19 +874,19 @@
         <v>0.6583334692618267</v>
       </c>
       <c r="D19">
-        <v>0.5605672639926587</v>
+        <v>0.4667117069342575</v>
       </c>
       <c r="E19">
-        <v>0.7560996745309947</v>
+        <v>0.8499552315893959</v>
       </c>
       <c r="F19">
         <v>0.1571604535087078</v>
       </c>
       <c r="G19">
-        <v>0.1044985748617532</v>
+        <v>0.05394317136067665</v>
       </c>
       <c r="H19">
-        <v>0.2098223321556625</v>
+        <v>0.260377735656739</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -900,19 +900,19 @@
         <v>0.685030232892659</v>
       </c>
       <c r="D20">
-        <v>0.5893248471546835</v>
+        <v>0.4974476768462271</v>
       </c>
       <c r="E20">
-        <v>0.7807356186306345</v>
+        <v>0.8726127889390908</v>
       </c>
       <c r="F20">
         <v>0.1762824249696147</v>
       </c>
       <c r="G20">
-        <v>0.117894052740874</v>
+        <v>0.06184121540128289</v>
       </c>
       <c r="H20">
-        <v>0.2346707971983555</v>
+        <v>0.2907236345379466</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -926,19 +926,19 @@
         <v>0.7092785386279885</v>
       </c>
       <c r="D21">
-        <v>0.6159555562389057</v>
+        <v>0.5263654931453863</v>
       </c>
       <c r="E21">
-        <v>0.8026015210170713</v>
+        <v>0.8921915841105907</v>
       </c>
       <c r="F21">
         <v>0.1960701378046621</v>
       </c>
       <c r="G21">
-        <v>0.1319578435724079</v>
+        <v>0.07041004110944385</v>
       </c>
       <c r="H21">
-        <v>0.2601824320369163</v>
+        <v>0.3217302344998804</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -952,19 +952,19 @@
         <v>0.7312889573539004</v>
       </c>
       <c r="D22">
-        <v>0.6405768500346936</v>
+        <v>0.5534932270082551</v>
       </c>
       <c r="E22">
-        <v>0.8220010646731073</v>
+        <v>0.9090846876995458</v>
       </c>
       <c r="F22">
         <v>0.2164089956272741</v>
       </c>
       <c r="G22">
-        <v>0.1466415492355168</v>
+        <v>0.07966480069942974</v>
       </c>
       <c r="H22">
-        <v>0.2861764420190315</v>
+        <v>0.3531531905551185</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -978,19 +978,19 @@
         <v>0.7512661132028564</v>
       </c>
       <c r="D23">
-        <v>0.6633165109604808</v>
+        <v>0.5788848928078003</v>
       </c>
       <c r="E23">
-        <v>0.839215715445232</v>
+        <v>0.9236473335979125</v>
       </c>
       <c r="F23">
         <v>0.2371842652563881</v>
       </c>
       <c r="G23">
-        <v>0.161892947395371</v>
+        <v>0.08961328224879445</v>
       </c>
       <c r="H23">
-        <v>0.3124755831174053</v>
+        <v>0.3847552482639818</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1004,19 +1004,19 @@
         <v>0.7694037912541376</v>
       </c>
       <c r="D24">
-        <v>0.684306053538056</v>
+        <v>0.6026122253306175</v>
       </c>
       <c r="E24">
-        <v>0.8545015289702192</v>
+        <v>0.9361953571776577</v>
       </c>
       <c r="F24">
         <v>0.2582830968939424</v>
       </c>
       <c r="G24">
-        <v>0.1776565141259882</v>
+        <v>0.1002549946687522</v>
       </c>
       <c r="H24">
-        <v>0.3389096796618965</v>
+        <v>0.4163111991191325</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1030,19 +1030,19 @@
         <v>0.7858822333795102</v>
       </c>
       <c r="D25">
-        <v>0.7036761035961712</v>
+        <v>0.6247582190041656</v>
       </c>
       <c r="E25">
-        <v>0.8680883631628493</v>
+        <v>0.9470062477548549</v>
       </c>
       <c r="F25">
         <v>0.2795962980192351</v>
       </c>
       <c r="G25">
-        <v>0.1938740377224997</v>
+        <v>0.1115806678376338</v>
       </c>
       <c r="H25">
-        <v>0.3653185583159704</v>
+        <v>0.4476119282008364</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1056,19 +1056,19 @@
         <v>0.8008669370928627</v>
       </c>
       <c r="D26">
-        <v>0.7215532806967584</v>
+        <v>0.6454121705564982</v>
       </c>
       <c r="E26">
-        <v>0.880180593488967</v>
+        <v>0.9563217036292272</v>
       </c>
       <c r="F26">
         <v>0.3010198313432233</v>
       </c>
       <c r="G26">
-        <v>0.2104853080263189</v>
+        <v>0.1235721656420907</v>
       </c>
       <c r="H26">
-        <v>0.3915543546601277</v>
+        <v>0.4784674970443559</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1082,19 +1082,19 @@
         <v>0.8145084508191788</v>
       </c>
       <c r="D27">
-        <v>0.7380582033968772</v>
+        <v>0.6646659658714676</v>
       </c>
       <c r="E27">
-        <v>0.8909586982414803</v>
+        <v>0.9643509357668899</v>
       </c>
       <c r="F27">
         <v>0.3224560226257095</v>
       </c>
       <c r="G27">
-        <v>0.2274288586854103</v>
+        <v>0.136202781302723</v>
       </c>
       <c r="H27">
-        <v>0.4174831865660088</v>
+        <v>0.5087092639486961</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1108,19 +1108,19 @@
         <v>0.8269428013422075</v>
       </c>
       <c r="D28">
-        <v>0.7533043163187657</v>
+        <v>0.6826113706962614</v>
       </c>
       <c r="E28">
-        <v>0.9005812863656494</v>
+        <v>0.9712742319881537</v>
       </c>
       <c r="F28">
         <v>0.343814478162365</v>
       </c>
       <c r="G28">
-        <v>0.2446427356524018</v>
+        <v>0.1494378628428371</v>
       </c>
       <c r="H28">
-        <v>0.4429862206723283</v>
+        <v>0.538191093481893</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1134,19 +1134,19 @@
         <v>0.838292297940637</v>
       </c>
       <c r="D29">
-        <v>0.767397306071687</v>
+        <v>0.6993381138774951</v>
       </c>
       <c r="E29">
-        <v>0.909187289809587</v>
+        <v>0.9772464820037788</v>
       </c>
       <c r="F29">
         <v>0.3650127235896455</v>
       </c>
       <c r="G29">
-        <v>0.2620652638848612</v>
+        <v>0.1632357025682683</v>
       </c>
       <c r="H29">
-        <v>0.4679601832944298</v>
+        <v>0.5667897446110227</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1160,19 +1160,19 @@
         <v>0.8486665382792236</v>
       </c>
       <c r="D30">
-        <v>0.7804349291163759</v>
+        <v>0.7149325843200421</v>
       </c>
       <c r="E30">
-        <v>0.9168981474420712</v>
+        <v>0.982400492238405</v>
       </c>
       <c r="F30">
         <v>0.3859765849387864</v>
       </c>
       <c r="G30">
-        <v>0.2796357853550495</v>
+        <v>0.177548617754662</v>
       </c>
       <c r="H30">
-        <v>0.4923173845225233</v>
+        <v>0.5944045521229108</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1186,19 +1186,19 @@
         <v>0.8581634993731267</v>
       </c>
       <c r="D31">
-        <v>0.7925071194508689</v>
+        <v>0.7294769947255014</v>
       </c>
       <c r="E31">
-        <v>0.9238198792953846</v>
+        <v>0.9868500040207521</v>
       </c>
       <c r="F31">
         <v>0.4066403394815257</v>
       </c>
       <c r="G31">
-        <v>0.2972953445948232</v>
+        <v>0.1923241495035889</v>
       </c>
       <c r="H31">
-        <v>0.5159853343682281</v>
+        <v>0.6209565294594624</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1212,19 +1212,19 @@
         <v>0.8668706382249897</v>
       </c>
       <c r="D32">
-        <v>0.803696278975676</v>
+        <v>0.7430488940963349</v>
       </c>
       <c r="E32">
-        <v>0.9300449974743034</v>
+        <v>0.9906923823536444</v>
       </c>
       <c r="F32">
         <v>0.4269466679645972</v>
       </c>
       <c r="G32">
-        <v>0.3149873024844758</v>
+        <v>0.2075063116235593</v>
       </c>
       <c r="H32">
-        <v>0.5389060334447187</v>
+        <v>0.6463870243056352</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1238,19 +1238,19 @@
         <v>0.8748659554580623</v>
       </c>
       <c r="D33">
-        <v>0.8140776802184075</v>
+        <v>0.755720935988339</v>
       </c>
       <c r="E33">
-        <v>0.9356542306977171</v>
+        <v>0.9940109749277857</v>
       </c>
       <c r="F33">
         <v>0.4468464416064418</v>
       </c>
       <c r="G33">
-        <v>0.3326578642196869</v>
+        <v>0.2230368299284022</v>
       </c>
       <c r="H33">
-        <v>0.5610350189931967</v>
+        <v>0.6706560532844815</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1264,19 +1264,19 @@
         <v>0.8822189948944728</v>
       </c>
       <c r="D34">
-        <v>0.8237199313537623</v>
+        <v>0.7675608303546804</v>
       </c>
       <c r="E34">
-        <v>0.9407180584351832</v>
+        <v>0.9968771594342651</v>
       </c>
       <c r="F34">
         <v>0.4662983771075705</v>
       </c>
       <c r="G34">
-        <v>0.3502565127960536</v>
+        <v>0.2388563230569974</v>
       </c>
       <c r="H34">
-        <v>0.5823402414190874</v>
+        <v>0.6937404311581437</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1290,19 +1290,19 @@
         <v>0.8889917651735436</v>
       </c>
       <c r="D35">
-        <v>0.8326854685501079</v>
+        <v>0.7786314237916097</v>
       </c>
       <c r="E35">
-        <v>0.9452980617969793</v>
+        <v>0.9993521065554776</v>
       </c>
       <c r="F35">
         <v>0.4852685913284632</v>
       </c>
       <c r="G35">
-        <v>0.3677363444797995</v>
+        <v>0.2549053875050823</v>
       </c>
       <c r="H35">
-        <v>0.6028008381771269</v>
+        <v>0.7156317951518442</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1316,19 +1316,19 @@
         <v>0.8952395781028454</v>
       </c>
       <c r="D36">
-        <v>0.8410310517877624</v>
+        <v>0.7889908665252827</v>
       </c>
       <c r="E36">
-        <v>0.9494481044179284</v>
+        <v>1.001488289680408</v>
       </c>
       <c r="F36">
         <v>0.5037300846364053</v>
       </c>
       <c r="G36">
-        <v>0.3850543072576857</v>
+        <v>0.271125560974115</v>
       </c>
       <c r="H36">
-        <v>0.6224058620151249</v>
+        <v>0.7363346082986957</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1342,19 +1342,19 @@
         <v>0.9010118038840241</v>
       </c>
       <c r="D37">
-        <v>0.8488082483810488</v>
+        <v>0.7986928350981926</v>
       </c>
       <c r="E37">
-        <v>0.9532153593869994</v>
+        <v>1.003330772669856</v>
       </c>
       <c r="F37">
         <v>0.5216621786008838</v>
       </c>
       <c r="G37">
-        <v>0.402171346978473</v>
+        <v>0.2874601486209586</v>
       </c>
       <c r="H37">
-        <v>0.6411530102232946</v>
+        <v>0.755864208580809</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1368,19 +1368,19 @@
         <v>0.9063525466553641</v>
       </c>
       <c r="D38">
-        <v>0.8560638942497466</v>
+        <v>0.8077867879403537</v>
       </c>
       <c r="E38">
-        <v>0.9566411990609817</v>
+        <v>1.004918305370375</v>
       </c>
       <c r="F38">
         <v>0.5390499300565987</v>
       </c>
       <c r="G38">
-        <v>0.4190524687262084</v>
+        <v>0.3038549058490337</v>
       </c>
       <c r="H38">
-        <v>0.659047391386989</v>
+        <v>0.7742449542641637</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1394,19 +1394,19 @@
         <v>0.9113012456480305</v>
       </c>
       <c r="D39">
-        <v>0.8628405271094206</v>
+        <v>0.816318237312355</v>
       </c>
       <c r="E39">
-        <v>0.9597619641866404</v>
+        <v>1.006284253983706</v>
       </c>
       <c r="F39">
         <v>0.5558835398198018</v>
       </c>
       <c r="G39">
-        <v>0.4356667229075685</v>
+        <v>0.3202585786718245</v>
       </c>
       <c r="H39">
-        <v>0.6761003567320351</v>
+        <v>0.791508500967779</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1420,19 +1420,19 @@
         <v>0.9158932081543402</v>
       </c>
       <c r="D40">
-        <v>0.8691767886298746</v>
+        <v>0.8243290258863876</v>
       </c>
       <c r="E40">
-        <v>0.9626096276788058</v>
+        <v>1.007457390422293</v>
       </c>
       <c r="F40">
         <v>0.572157770737991</v>
       </c>
       <c r="G40">
-        <v>0.4519871266631508</v>
+        <v>0.3366233083513042</v>
       </c>
       <c r="H40">
-        <v>0.6923284148128312</v>
+        <v>0.8076922331246779</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -1446,19 +1446,19 @@
         <v>0.9201600807934496</v>
       </c>
       <c r="D41">
-        <v>0.8751077945829688</v>
+        <v>0.8318575998209072</v>
       </c>
       <c r="E41">
-        <v>0.9652123670039303</v>
+        <v>1.008462561765992</v>
       </c>
       <c r="F41">
         <v>0.5878713864144517</v>
       </c>
       <c r="G41">
-        <v>0.4679905316392983</v>
+        <v>0.3529049110551511</v>
       </c>
       <c r="H41">
-        <v>0.7077522411896051</v>
+        <v>0.8228378617737523</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -1472,19 +1472,19 @@
         <v>0.9241302654641174</v>
       </c>
       <c r="D42">
-        <v>0.8806654733165985</v>
+        <v>0.8389392728549804</v>
       </c>
       <c r="E42">
-        <v>0.9675950576116362</v>
+        <v>1.009321258073254</v>
       </c>
       <c r="F42">
         <v>0.603026618964475</v>
       </c>
       <c r="G42">
-        <v>0.4836574490165229</v>
+        <v>0.3690630458664889</v>
       </c>
       <c r="H42">
-        <v>0.7223957889124271</v>
+        <v>0.8369901920624611</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -1498,19 +1498,19 @@
         <v>0.9278292860519359</v>
       </c>
       <c r="D43">
-        <v>0.8858788737370933</v>
+        <v>0.8456064779148443</v>
       </c>
       <c r="E43">
-        <v>0.9697796983667786</v>
+        <v>1.010052094189027</v>
       </c>
       <c r="F43">
         <v>0.6176286715729775</v>
       </c>
       <c r="G43">
-        <v>0.4989718421204737</v>
+        <v>0.38506128584607</v>
       </c>
       <c r="H43">
-        <v>0.7362855010254813</v>
+        <v>0.850196057299885</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -1524,19 +1524,19 @@
         <v>0.9312801115134846</v>
       </c>
       <c r="D44">
-        <v>0.8907744444948001</v>
+        <v>0.8518890041568631</v>
       </c>
       <c r="E44">
-        <v>0.971785778532169</v>
+        <v>1.010671218870106</v>
       </c>
       <c r="F44">
         <v>0.6316852594441843</v>
       </c>
       <c r="G44">
-        <v>0.513920896071216</v>
+        <v>0.4008671072331665</v>
       </c>
       <c r="H44">
-        <v>0.7494496228171525</v>
+        <v>0.8625034116552021</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -1550,19 +1550,19 @@
         <v>0.9345034404599992</v>
       </c>
       <c r="D45">
-        <v>0.8953762863474017</v>
+        <v>0.8578142183993083</v>
       </c>
       <c r="E45">
-        <v>0.9736305945725967</v>
+        <v>1.01119266252069</v>
       </c>
       <c r="F45">
         <v>0.6452061909496449</v>
       </c>
       <c r="G45">
-        <v>0.5284947728705426</v>
+        <v>0.4164518115146043</v>
       </c>
       <c r="H45">
-        <v>0.7619176090287473</v>
+        <v>0.8739605703846856</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -1576,19 +1576,19 @@
         <v>0.9375179518514138</v>
       </c>
       <c r="D46">
-        <v>0.8997063797952997</v>
+        <v>0.86340727062143</v>
       </c>
       <c r="E46">
-        <v>0.975329523907528</v>
+        <v>1.011628633081398</v>
       </c>
       <c r="F46">
         <v>0.6582029893617393</v>
       </c>
       <c r="G46">
-        <v>0.5426863591801219</v>
+        <v>0.4317903942057691</v>
       </c>
       <c r="H46">
-        <v>0.7737196195433567</v>
+        <v>0.8846155845177094</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -1602,19 +1602,19 @@
         <v>0.9403405259144229</v>
       </c>
       <c r="D47">
-        <v>0.9037847900956664</v>
+        <v>0.8686912837096602</v>
       </c>
       <c r="E47">
-        <v>0.9768962617331793</v>
+        <v>1.011989768119186</v>
       </c>
       <c r="F47">
         <v>0.6706885544672098</v>
       </c>
       <c r="G47">
-        <v>0.5564910128803696</v>
+        <v>0.4468613729570031</v>
       </c>
       <c r="H47">
-        <v>0.7848860960540499</v>
+        <v>0.8945157359774164</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -1628,19 +1628,19 @@
         <v>0.9429864389306831</v>
       </c>
       <c r="D48">
-        <v>0.9076298517039529</v>
+        <v>0.8736875279662919</v>
       </c>
       <c r="E48">
-        <v>0.9783430261574133</v>
+        <v>1.012285349895074</v>
       </c>
       <c r="F48">
         <v>0.682676862545901</v>
       </c>
       <c r="G48">
-        <v>0.5699063133765994</v>
+        <v>0.4616465861740698</v>
       </c>
       <c r="H48">
-        <v>0.7954474117152026</v>
+        <v>0.9037071389177321</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -1654,19 +1654,19 @@
         <v>0.9454695351112938</v>
       </c>
       <c r="D49">
-        <v>0.9112583340903312</v>
+        <v>0.878415581110207</v>
       </c>
       <c r="E49">
-        <v>0.9796807361322565</v>
+        <v>1.012523489112381</v>
       </c>
       <c r="F49">
         <v>0.6941827026299194</v>
       </c>
       <c r="G49">
-        <v>0.5829318195738022</v>
+        <v>0.4761309718399298</v>
       </c>
       <c r="H49">
-        <v>0.8054335856860366</v>
+        <v>0.9122344334199091</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -1680,19 +1680,19 @@
         <v>0.9478023783843095</v>
       </c>
       <c r="D50">
-        <v>0.9146855907523134</v>
+        <v>0.8828934746255972</v>
       </c>
       <c r="E50">
-        <v>0.9809191660163056</v>
+        <v>1.012711282143022</v>
       </c>
       <c r="F50">
         <v>0.7052214465857818</v>
       </c>
       <c r="G50">
-        <v>0.5955688384983376</v>
+        <v>0.4903023347343912</v>
       </c>
       <c r="H50">
-        <v>0.8148740546732259</v>
+        <v>0.9201405584371724</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -1706,19 +1706,19 @@
         <v>0.9499963865733911</v>
       </c>
       <c r="D51">
-        <v>0.9179256931064779</v>
+        <v>0.8871378273782411</v>
       </c>
       <c r="E51">
-        <v>0.9820670800403044</v>
+        <v>1.012854945768541</v>
       </c>
       <c r="F51">
         <v>0.7158088503481832</v>
       </c>
       <c r="G51">
-        <v>0.607820206716337</v>
+        <v>0.5041511088297645</v>
       </c>
       <c r="H51">
-        <v>0.8237974939800294</v>
+        <v>0.9274665918666019</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -1732,19 +1732,19 @@
         <v>0.9520619501360569</v>
       </c>
       <c r="D52">
-        <v>0.9209915508004861</v>
+        <v>0.8911639674383383</v>
       </c>
       <c r="E52">
-        <v>0.9831323494716276</v>
+        <v>1.012959932833776</v>
       </c>
       <c r="F52">
         <v>0.7259608835445561</v>
       </c>
       <c r="G52">
-        <v>0.6196900859883567</v>
+        <v>0.5176701203344054</v>
       </c>
       <c r="H52">
-        <v>0.8322316811007555</v>
+        <v>0.9342516467547068</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -1758,19 +1758,19 @@
         <v>0.9540085373567139</v>
       </c>
       <c r="D53">
-        <v>0.9238950198471674</v>
+        <v>0.8949860430380027</v>
       </c>
       <c r="E53">
-        <v>0.9841220548662604</v>
+        <v>1.013031031675425</v>
       </c>
       <c r="F53">
         <v>0.7356935847549534</v>
       </c>
       <c r="G53">
-        <v>0.6311837740048614</v>
+        <v>0.5308543556847729</v>
       </c>
       <c r="H53">
-        <v>0.8402033955050454</v>
+        <v>0.9405328138251339</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -1784,19 +1784,19 @@
         <v>0.9558447876495498</v>
       </c>
       <c r="D54">
-        <v>0.9266469998489545</v>
+        <v>0.898617123560383</v>
       </c>
       <c r="E54">
-        <v>0.9850425754501452</v>
+        <v>1.013072451738717</v>
       </c>
       <c r="F54">
         <v>0.7450229397271021</v>
       </c>
       <c r="G54">
-        <v>0.6423075305603578</v>
+        <v>0.5437007377602833</v>
       </c>
       <c r="H54">
-        <v>0.8477383488938464</v>
+        <v>0.9463451416939209</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -1810,19 +1810,19 @@
         <v>0.9575785944161194</v>
       </c>
       <c r="D55">
-        <v>0.9292575214555236</v>
+        <v>0.9020692914133517</v>
       </c>
       <c r="E55">
-        <v>0.9858996673767151</v>
+        <v>1.013087897418887</v>
       </c>
       <c r="F55">
         <v>0.7539647799910881</v>
       </c>
       <c r="G55">
-        <v>0.6530684191354631</v>
+        <v>0.5562079127140631</v>
       </c>
       <c r="H55">
-        <v>0.8548611408467132</v>
+        <v>0.9517216472681131</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -1836,19 +1836,19 @@
         <v>0.9592171787188531</v>
       </c>
       <c r="D56">
-        <v>0.9317358250812756</v>
+        <v>0.9053537255892011</v>
       </c>
       <c r="E56">
-        <v>0.9866985323564307</v>
+        <v>1.013080631848505</v>
       </c>
       <c r="F56">
         <v>0.7625346994755233</v>
       </c>
       <c r="G56">
-        <v>0.66347416355468</v>
+        <v>0.5683760490706705</v>
       </c>
       <c r="H56">
-        <v>0.8615952353963666</v>
+        <v>0.9566933498803761</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -1862,19 +1862,19 @@
         <v>0.9607671548716183</v>
       </c>
       <c r="D57">
-        <v>0.9340904318026757</v>
+        <v>0.9084807776564908</v>
       </c>
       <c r="E57">
-        <v>0.987443877940561</v>
+        <v>1.013053532086746</v>
       </c>
       <c r="F57">
         <v>0.7707479869040317</v>
       </c>
       <c r="G57">
-        <v>0.6735330191614022</v>
+        <v>0.5802066501284778</v>
       </c>
       <c r="H57">
-        <v>0.8679629546466612</v>
+        <v>0.9612893236795855</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -1888,19 +1888,19 @@
         <v>0.9622345889090655</v>
       </c>
       <c r="D58">
-        <v>0.9363292072584483</v>
+        <v>0.9114600408738556</v>
       </c>
       <c r="E58">
-        <v>0.9881399705596828</v>
+        <v>1.013009136944276</v>
       </c>
       <c r="F58">
         <v>0.7786195719373805</v>
       </c>
       <c r="G58">
-        <v>0.6832536577892634</v>
+        <v>0.5917023802070709</v>
       </c>
       <c r="H58">
-        <v>0.8739854860854976</v>
+        <v>0.9655367636676901</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -1914,19 +1914,19 @@
         <v>0.9636250507751988</v>
       </c>
       <c r="D59">
-        <v>0.9384594192878398</v>
+        <v>0.9143004130599752</v>
       </c>
       <c r="E59">
-        <v>0.9887906822625577</v>
+        <v>1.012949688490422</v>
       </c>
       <c r="F59">
         <v>0.7861639832149189</v>
       </c>
       <c r="G59">
-        <v>0.6926450656996007</v>
+        <v>0.6028669048848951</v>
       </c>
       <c r="H59">
-        <v>0.879682900730237</v>
+        <v>0.9694610615449426</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -1940,19 +1940,19 @@
         <v>0.9649436609661156</v>
       </c>
       <c r="D60">
-        <v>0.940487789963129</v>
+        <v>0.9170101538002619</v>
       </c>
       <c r="E60">
-        <v>0.9893995319691022</v>
+        <v>1.012877168131969</v>
       </c>
       <c r="F60">
         <v>0.7933953166336031</v>
       </c>
       <c r="G60">
-        <v>0.7017164535887338</v>
+        <v>0.6137047450656593</v>
       </c>
       <c r="H60">
-        <v>0.8850741796784724</v>
+        <v>0.9730858882015468</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -1966,19 +1966,19 @@
         <v>0.9661951322701186</v>
       </c>
       <c r="D61">
-        <v>0.9424205426016312</v>
+        <v>0.9195969365198835</v>
       </c>
       <c r="E61">
-        <v>0.9899697219386059</v>
+        <v>1.012793328020354</v>
       </c>
       <c r="F61">
         <v>0.800327212379871</v>
       </c>
       <c r="G61">
-        <v>0.7104771777372879</v>
+        <v>0.6242211444804081</v>
       </c>
       <c r="H61">
-        <v>0.8901772470224542</v>
+        <v>0.976433280279334</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -1992,19 +1992,19 @@
         <v>0.9673838071686084</v>
       </c>
       <c r="D62">
-        <v>0.9442634442790003</v>
+        <v>0.9220678959049766</v>
       </c>
       <c r="E62">
-        <v>0.9905041700582164</v>
+        <v>1.01269971843224</v>
       </c>
       <c r="F62">
         <v>0.8069728393963701</v>
       </c>
       <c r="G62">
-        <v>0.7189366713693597</v>
+        <v>0.6344219500634297</v>
       </c>
       <c r="H62">
-        <v>0.8950090074233805</v>
+        <v>0.9795237287293105</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -2018,19 +2018,19 @@
         <v>0.9685136913917546</v>
       </c>
       <c r="D63">
-        <v>0.9460218443089778</v>
+        <v>0.9244296711095121</v>
       </c>
       <c r="E63">
-        <v>0.9910055384745313</v>
+        <v>1.012597711673997</v>
       </c>
       <c r="F63">
         <v>0.8133448861204609</v>
       </c>
       <c r="G63">
-        <v>0.7271043853054965</v>
+        <v>0.6443135045231306</v>
       </c>
       <c r="H63">
-        <v>0.8995853869354252</v>
+        <v>0.9823762677177911</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -2044,19 +2044,19 @@
         <v>0.9695884840625054</v>
       </c>
       <c r="D64">
-        <v>0.9477007091042392</v>
+        <v>0.9266884451443036</v>
       </c>
       <c r="E64">
-        <v>0.9914762590207716</v>
+        <v>1.012488522980707</v>
       </c>
       <c r="F64">
         <v>0.8194555564737278</v>
       </c>
       <c r="G64">
-        <v>0.7349897370248673</v>
+        <v>0.6539025503539611</v>
       </c>
       <c r="H64">
-        <v>0.9039213759225884</v>
+        <v>0.9850085625934946</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -2070,19 +2070,19 @@
         <v>0.9706116048098726</v>
       </c>
       <c r="D65">
-        <v>0.9493046537880322</v>
+        <v>0.9288499808070655</v>
       </c>
       <c r="E65">
-        <v>0.9919185558317131</v>
+        <v>1.01237322881268</v>
       </c>
       <c r="F65">
         <v>0.8253165702111868</v>
       </c>
       <c r="G65">
-        <v>0.742602067294181</v>
+        <v>0.6631961444938554</v>
       </c>
       <c r="H65">
-        <v>0.9080310731281925</v>
+        <v>0.9874369959285181</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -2096,19 +2096,19 @@
         <v>0.9715862181865589</v>
       </c>
       <c r="D66">
-        <v>0.9508379708863226</v>
+        <v>0.9309196534780958</v>
       </c>
       <c r="E66">
-        <v>0.9923344654867952</v>
+        <v>1.012252782895022</v>
       </c>
       <c r="F66">
         <v>0.8309391668556981</v>
       </c>
       <c r="G66">
-        <v>0.7499506035702632</v>
+        <v>0.6722015828162458</v>
       </c>
       <c r="H66">
-        <v>0.911927730141133</v>
+        <v>0.9896767508951505</v>
       </c>
     </row>
     <row r="67" spans="1:8">
@@ -2122,19 +2122,19 @@
         <v>0.9725152556859733</v>
       </c>
       <c r="D67">
-        <v>0.9523046563946053</v>
+        <v>0.9329024810748919</v>
       </c>
       <c r="E67">
-        <v>0.9927258549773413</v>
+        <v>1.012128030297055</v>
       </c>
       <c r="F67">
         <v>0.8363341125477481</v>
       </c>
       <c r="G67">
-        <v>0.7570444294368444</v>
+        <v>0.6809263336503768</v>
       </c>
       <c r="H67">
-        <v>0.9156237956586519</v>
+        <v>0.9917418914451195</v>
       </c>
     </row>
     <row r="68" spans="1:8">
@@ -2148,19 +2148,19 @@
         <v>0.973401435618753</v>
       </c>
       <c r="D68">
-        <v>0.9537084334819634</v>
+        <v>0.9348031514306453</v>
       </c>
       <c r="E68">
-        <v>0.9930944377555426</v>
+        <v>1.011999719806861</v>
       </c>
       <c r="F68">
         <v>0.841511709233964</v>
       </c>
       <c r="G68">
-        <v>0.7638924593918345</v>
+        <v>0.6893779795433902</v>
       </c>
       <c r="H68">
-        <v>0.9191309590760935</v>
+        <v>0.9936454389245378</v>
       </c>
     </row>
     <row r="69" spans="1:8">
@@ -2174,19 +2174,19 @@
         <v>0.9742472810783666</v>
       </c>
       <c r="D69">
-        <v>0.9550527740668752</v>
+        <v>0.9366260473358435</v>
       </c>
       <c r="E69">
-        <v>0.9934417880898579</v>
+        <v>1.01186851482089</v>
       </c>
       <c r="F69">
         <v>0.846481805700225</v>
       </c>
       <c r="G69">
-        <v>0.7705034183573554</v>
+        <v>0.6975641665082004</v>
       </c>
       <c r="H69">
-        <v>0.9224601930430947</v>
+        <v>0.9953994448922496</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -2200,19 +2200,19 @@
         <v>0.9750551361986803</v>
       </c>
       <c r="D70">
-        <v>0.9563409184743519</v>
+        <v>0.9383752694589966</v>
       </c>
       <c r="E70">
-        <v>0.9937693539230088</v>
+        <v>1.011735002938364</v>
       </c>
       <c r="F70">
         <v>0.8512538100279479</v>
       </c>
       <c r="G70">
-        <v>0.7768858253398669</v>
+        <v>0.7054925600393094</v>
       </c>
       <c r="H70">
-        <v>0.9256217947160288</v>
+        <v>0.9970150600165864</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -2226,19 +2226,19 @@
         <v>0.9758271808829662</v>
       </c>
       <c r="D71">
-        <v>0.9575758933618065</v>
+        <v>0.9400546573414932</v>
       </c>
       <c r="E71">
-        <v>0.9940784684041258</v>
+        <v>1.011599704424439</v>
       </c>
       <c r="F71">
         <v>0.8558367031158722</v>
       </c>
       <c r="G71">
-        <v>0.7830479807208418</v>
+        <v>0.7131708072216126</v>
       </c>
       <c r="H71">
-        <v>0.9286254255109027</v>
+        <v>0.9985025990101318</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -2252,19 +2252,19 @@
         <v>0.9765654441633379</v>
       </c>
       <c r="D72">
-        <v>0.958760528081379</v>
+        <v>0.9416678086426985</v>
       </c>
       <c r="E72">
-        <v>0.9943703602452968</v>
+        <v>1.011463079683977</v>
       </c>
       <c r="F72">
         <v>0.8602390529653683</v>
       </c>
       <c r="G72">
-        <v>0.7889979567090091</v>
+        <v>0.7206065043029042</v>
       </c>
       <c r="H72">
-        <v>0.9314801492217275</v>
+        <v>0.9998716016278324</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -2278,19 +2278,19 @@
         <v>0.9772718163316009</v>
       </c>
       <c r="D73">
-        <v>0.9598974696289062</v>
+        <v>0.9432180967943193</v>
       </c>
       <c r="E73">
-        <v>0.9946461630342955</v>
+        <v>1.011325535868882</v>
       </c>
       <c r="F73">
         <v>0.8644690294757313</v>
       </c>
       <c r="G73">
-        <v>0.7947435905327632</v>
+        <v>0.7278071691475138</v>
       </c>
       <c r="H73">
-        <v>0.9341944684186995</v>
+        <v>1.001130889803949</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -2304,19 +2304,19 @@
         <v>0.9779480599666964</v>
       </c>
       <c r="D74">
-        <v>0.9609891963141571</v>
+        <v>0.9447086872077194</v>
       </c>
       <c r="E74">
-        <v>0.9949069236192357</v>
+        <v>1.011187432725674</v>
       </c>
       <c r="F74">
         <v>0.8685344195379124</v>
       </c>
       <c r="G74">
-        <v>0.8002924799956492</v>
+        <v>0.7347802180350766</v>
       </c>
       <c r="H74">
-        <v>0.9367763590801756</v>
+        <v>1.002288621040748</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -2330,19 +2330,19 @@
         <v>0.9785958199700194</v>
       </c>
       <c r="D75">
-        <v>0.9620380302730854</v>
+        <v>0.9461425521640288</v>
       </c>
       <c r="E75">
-        <v>0.9951536096669534</v>
+        <v>1.01104908777601</v>
       </c>
       <c r="F75">
         <v>0.8724426422514001</v>
       </c>
       <c r="G75">
-        <v>0.8056519810588239</v>
+        <v>0.7415329463139506</v>
       </c>
       <c r="H75">
-        <v>0.9392333034439764</v>
+        <v>1.00335233818885</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -2356,19 +2356,19 @@
         <v>0.9792166327076363</v>
       </c>
       <c r="D76">
-        <v>0.9630461489304905</v>
+        <v>0.9475224845044304</v>
       </c>
       <c r="E76">
-        <v>0.9953871164847821</v>
+        <v>1.010910780910842</v>
       </c>
       <c r="F76">
         <v>0.8762007641201703</v>
       </c>
       <c r="G76">
-        <v>0.810829207152001</v>
+        <v>0.7480725124625585</v>
       </c>
       <c r="H76">
-        <v>0.9415723210883397</v>
+        <v>1.004329015777782</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -2382,19 +2382,19 @@
         <v>0.9798119343476441</v>
       </c>
       <c r="D77">
-        <v>0.9640155955104787</v>
+        <v>0.9488511102267998</v>
       </c>
       <c r="E77">
-        <v>0.9956082731848096</v>
+        <v>1.010772758468488</v>
       </c>
       <c r="F77">
         <v>0.8798155141103828</v>
       </c>
       <c r="G77">
-        <v>0.8158310299487268</v>
+        <v>0.754405925153537</v>
       </c>
       <c r="H77">
-        <v>0.9437999982720389</v>
+        <v>1.005225103067229</v>
       </c>
     </row>
     <row r="78" spans="1:8">
@@ -2408,19 +2408,19 @@
         <v>0.9803830684713849</v>
       </c>
       <c r="D78">
-        <v>0.9649482886823069</v>
+        <v>0.950130900084792</v>
       </c>
       <c r="E78">
-        <v>0.9958178482604629</v>
+        <v>1.010635236857978</v>
       </c>
       <c r="F78">
         <v>0.8832932984753704</v>
       </c>
       <c r="G78">
-        <v>0.8206640813729856</v>
+        <v>0.7605400329546962</v>
       </c>
       <c r="H78">
-        <v>0.9459225155777552</v>
+        <v>1.006046563996045</v>
       </c>
     </row>
     <row r="79" spans="1:8">
@@ -2434,19 +2434,19 @@
         <v>0.9809312930288066</v>
       </c>
       <c r="D79">
-        <v>0.96584603142042</v>
+        <v>0.9513641802763689</v>
       </c>
       <c r="E79">
-        <v>0.9960165546371931</v>
+        <v>1.010498405781244</v>
       </c>
       <c r="F79">
         <v>0.8866402152729398</v>
       </c>
       <c r="G79">
-        <v>0.8253347566323048</v>
+        <v>0.7664815163372951</v>
       </c>
       <c r="H79">
-        <v>0.9479456739135748</v>
+        <v>1.006798914208584</v>
       </c>
     </row>
     <row r="80" spans="1:8">
@@ -2460,19 +2460,19 @@
         <v>0.9814577867008233</v>
       </c>
       <c r="D80">
-        <v>0.9667105191496854</v>
+        <v>0.952553142300593</v>
       </c>
       <c r="E80">
-        <v>0.9962050542519612</v>
+        <v>1.010362431101054</v>
       </c>
       <c r="F80">
         <v>0.8898620685165171</v>
       </c>
       <c r="G80">
-        <v>0.8298492180978611</v>
+        <v>0.7722368816959514</v>
       </c>
       <c r="H80">
-        <v>0.9498749189351731</v>
+        <v>1.007487255337083</v>
       </c>
     </row>
     <row r="81" spans="1:8">
@@ -2486,19 +2486,19 @@
         <v>0.9819636547249266</v>
       </c>
       <c r="D81">
-        <v>0.9675433472398252</v>
+        <v>0.9536998520541278</v>
       </c>
       <c r="E81">
-        <v>0.9963839622100281</v>
+        <v>1.010227457395726</v>
       </c>
       <c r="F81">
         <v>0.8929643819156271</v>
       </c>
       <c r="G81">
-        <v>0.8342133998748115</v>
+        <v>0.7778124571156285</v>
       </c>
       <c r="H81">
-        <v>0.9517153639564427</v>
+        <v>1.008116306715626</v>
       </c>
     </row>
     <row r="82" spans="1:8">
@@ -2512,19 +2512,19 @@
         <v>0.9824499342344616</v>
       </c>
       <c r="D82">
-        <v>0.9683460179068127</v>
+        <v>0.9548062582322698</v>
       </c>
       <c r="E82">
-        <v>0.9965538505621104</v>
+        <v>1.010093610236653</v>
       </c>
       <c r="F82">
         <v>0.8959524121729321</v>
       </c>
       <c r="G82">
-        <v>0.8384330129263653</v>
+        <v>0.7832143896496612</v>
       </c>
       <c r="H82">
-        <v>0.9534718114194989</v>
+        <v>1.008690434696203</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -2538,19 +2538,19 @@
         <v>0.9829175991567835</v>
       </c>
       <c r="D83">
-        <v>0.9691199465733868</v>
+        <v>0.955874200093326</v>
       </c>
       <c r="E83">
-        <v>0.9967152517401801</v>
+        <v>1.009960998220241</v>
       </c>
       <c r="F83">
         <v>0.898831161814882</v>
       </c>
       <c r="G83">
-        <v>0.8425135506331942</v>
+        <v>0.7884486438987739</v>
       </c>
       <c r="H83">
-        <v>0.9551487729965698</v>
+        <v>1.00921367973099</v>
       </c>
     </row>
     <row r="84" spans="1:8">
@@ -2564,19 +2564,19 @@
         <v>0.9833675647109053</v>
       </c>
       <c r="D84">
-        <v>0.9698664677358342</v>
+        <v>0.9569054146397661</v>
       </c>
       <c r="E84">
-        <v>0.9968686616859763</v>
+        <v>1.009829714782045</v>
       </c>
       <c r="F84">
         <v>0.9016053915412098</v>
       </c>
       <c r="G84">
-        <v>0.8464602946858215</v>
+        <v>0.7935210017046488</v>
       </c>
       <c r="H84">
-        <v>0.956750488396598</v>
+        <v>1.009689781377771</v>
       </c>
     </row>
     <row r="85" spans="1:8">
@@ -2590,19 +2590,19 @@
         <v>0.9838006915411446</v>
       </c>
       <c r="D85">
-        <v>0.9705868403796976</v>
+        <v>0.9579015432647083</v>
       </c>
       <c r="E85">
-        <v>0.9970145427025916</v>
+        <v>1.009699839817581</v>
       </c>
       <c r="F85">
         <v>0.9042796320852764</v>
       </c>
       <c r="G85">
-        <v>0.8502783212218519</v>
+        <v>0.7984370627929643</v>
       </c>
       <c r="H85">
-        <v>0.9582809429487009</v>
+        <v>1.010122201377588</v>
       </c>
     </row>
     <row r="86" spans="1:8">
@@ -2616,19 +2616,19 @@
         <v>0.9842177895196215</v>
       </c>
       <c r="D86">
-        <v>0.9712822529830286</v>
+        <v>0.9588641379078995</v>
       </c>
       <c r="E86">
-        <v>0.9971533260562143</v>
+        <v>1.009571441131343</v>
       </c>
       <c r="F86">
         <v>0.9068581955828419</v>
       </c>
       <c r="G86">
-        <v>0.8539725071324615</v>
+        <v>0.8032022462200964</v>
       </c>
       <c r="H86">
-        <v>0.9597438840332222</v>
+        <v>1.010514144945587</v>
       </c>
     </row>
     <row r="87" spans="1:8">
@@ -2642,19 +2642,19 @@
         <v>0.9846196212472073</v>
       </c>
       <c r="D87">
-        <v>0.9719538281421911</v>
+        <v>0.9597946667613756</v>
       </c>
       <c r="E87">
-        <v>0.9972854143522234</v>
+        <v>1.009444575733039</v>
       </c>
       <c r="F87">
         <v>0.9093451864513648</v>
       </c>
       <c r="G87">
-        <v>0.8575475364736207</v>
+        <v>0.8078217924949863</v>
       </c>
       <c r="H87">
-        <v>0.9611428364291088</v>
+        <v>1.010868580407743</v>
       </c>
     </row>
     <row r="88" spans="1:8">
@@ -2668,19 +2668,19 @@
         <v>0.9850069052796118</v>
       </c>
       <c r="D88">
-        <v>0.9726026268519546</v>
+        <v>0.9606945195614037</v>
       </c>
       <c r="E88">
-        <v>0.9974111837072689</v>
+        <v>1.00931929099782</v>
       </c>
       <c r="F88">
         <v>0.911744511785605</v>
       </c>
       <c r="G88">
-        <v>0.8610079069272542</v>
+        <v>0.8123007662632373</v>
       </c>
       <c r="H88">
-        <v>0.9624811166439559</v>
+        <v>1.011188257307973</v>
       </c>
     </row>
     <row r="89" spans="1:8">
@@ -2694,19 +2694,19 @@
         <v>0.9853803191027057</v>
       </c>
       <c r="D89">
-        <v>0.9732296524687035</v>
+        <v>0.9615650125000614</v>
       </c>
       <c r="E89">
-        <v>0.997530985736708</v>
+        <v>1.00919562570535</v>
       </c>
       <c r="F89">
         <v>0.914059891278214</v>
       </c>
       <c r="G89">
-        <v>0.8643579362660603</v>
+        <v>0.8166440594543928</v>
       </c>
       <c r="H89">
-        <v>0.9637618462903677</v>
+        <v>1.011475723102035</v>
       </c>
     </row>
     <row r="90" spans="1:8">
@@ -2720,19 +2720,19 @@
         <v>0.9857405018788503</v>
       </c>
       <c r="D90">
-        <v>0.9738358543829444</v>
+        <v>0.9624073927868747</v>
       </c>
       <c r="E90">
-        <v>0.9976451493747562</v>
+        <v>1.009073610970826</v>
       </c>
       <c r="F90">
         <v>0.9162948666762926</v>
       </c>
       <c r="G90">
-        <v>0.8676017687831724</v>
+        <v>0.820856394805777</v>
       </c>
       <c r="H90">
-        <v>0.9649879645694127</v>
+        <v>1.011733338546808</v>
       </c>
     </row>
     <row r="91" spans="1:8">
@@ -2746,19 +2746,19 @@
         <v>0.9860880569839215</v>
       </c>
       <c r="D91">
-        <v>0.9744221314249141</v>
+        <v>0.963222842888267</v>
       </c>
       <c r="E91">
-        <v>0.997753982542929</v>
+        <v>1.008953271079576</v>
       </c>
       <c r="F91">
         <v>0.9184528107866569</v>
       </c>
       <c r="G91">
-        <v>0.8707433816543482</v>
+        <v>0.8249423296873319</v>
       </c>
       <c r="H91">
-        <v>0.9661622399189655</v>
+        <v>1.011963291885982</v>
       </c>
     </row>
     <row r="92" spans="1:8">
@@ -2772,19 +2772,19 @@
         <v>0.9864235543528643</v>
       </c>
       <c r="D92">
-        <v>0.9749893350249638</v>
+        <v>0.9640124844701793</v>
       </c>
       <c r="E92">
-        <v>0.9978577736807649</v>
+        <v>1.008834624235549</v>
       </c>
       <c r="F92">
         <v>0.920536936043866</v>
       </c>
       <c r="G92">
-        <v>0.8737865912060344</v>
+        <v>0.8289062601617161</v>
       </c>
       <c r="H92">
-        <v>0.9672872808816976</v>
+        <v>1.012167611926016</v>
       </c>
     </row>
     <row r="93" spans="1:8">
@@ -2798,19 +2798,19 @@
         <v>0.986747532649927</v>
       </c>
       <c r="D93">
-        <v>0.975538272148445</v>
+        <v>0.9647773820670222</v>
       </c>
       <c r="E93">
-        <v>0.9979567931514089</v>
+        <v>1.008717683232832</v>
       </c>
       <c r="F93">
         <v>0.9225503026560212</v>
       </c>
       <c r="G93">
-        <v>0.8767350590675776</v>
+        <v>0.8327524252226718</v>
       </c>
       <c r="H93">
-        <v>0.9683655462444648</v>
+        <v>1.012348180089371</v>
       </c>
     </row>
     <row r="94" spans="1:8">
@@ -2824,19 +2824,19 @@
         <v>0.9870605012782363</v>
       </c>
       <c r="D94">
-        <v>0.9760697080230919</v>
+        <v>0.9655185464981532</v>
       </c>
       <c r="E94">
-        <v>0.9980512945333807</v>
+        <v>1.008602456058319</v>
       </c>
       <c r="F94">
         <v>0.9244958263439734</v>
       </c>
       <c r="G94">
-        <v>0.8795922981901002</v>
+        <v>0.8364849111623819</v>
       </c>
       <c r="H94">
-        <v>0.9693993544978466</v>
+        <v>1.012506741525565</v>
       </c>
     </row>
     <row r="95" spans="1:8">
@@ -2850,19 +2850,19 @@
         <v>0.9873629422420165</v>
       </c>
       <c r="D95">
-        <v>0.9765843686753056</v>
+        <v>0.9662369380512633</v>
       </c>
       <c r="E95">
-        <v>0.9981415158087273</v>
+        <v>1.00848894643277</v>
       </c>
       <c r="F95">
         <v>0.9263762856899642</v>
       </c>
       <c r="G95">
-        <v>0.8823616787182396</v>
+        <v>0.840107656025384</v>
       </c>
       <c r="H95">
-        <v>0.9703908926616889</v>
+        <v>1.012644915354544</v>
       </c>
     </row>
     <row r="96" spans="1:8">
@@ -2876,19 +2876,19 @@
         <v>0.9876553118735428</v>
       </c>
       <c r="D96">
-        <v>0.9770829432903221</v>
+        <v>0.9669334694504302</v>
       </c>
       <c r="E96">
-        <v>0.9982276804567636</v>
+        <v>1.008377154296656</v>
       </c>
       <c r="F96">
         <v>0.9281943291118981</v>
       </c>
       <c r="G96">
-        <v>0.8850464337041153</v>
+        <v>0.8436244541126436</v>
       </c>
       <c r="H96">
-        <v>0.971342224519681</v>
+        <v>1.012764204111153</v>
       </c>
     </row>
     <row r="97" spans="1:8">
@@ -2902,19 +2902,19 @@
         <v>0.9879380424358302</v>
       </c>
       <c r="D97">
-        <v>0.9775660864099529</v>
+        <v>0.9676090086251107</v>
       </c>
       <c r="E97">
-        <v>0.9983099984617074</v>
+        <v>1.00826707624655</v>
       </c>
       <c r="F97">
         <v>0.929952481479442</v>
       </c>
       <c r="G97">
-        <v>0.8876496646555952</v>
+        <v>0.8470389605047024</v>
       </c>
       <c r="H97">
-        <v>0.9722552983032887</v>
+        <v>1.012866002454182</v>
       </c>
     </row>
     <row r="98" spans="1:8">
@@ -2928,19 +2928,19 @@
         <v>0.9882115436110671</v>
       </c>
       <c r="D98">
-        <v>0.9780344199804177</v>
+        <v>0.9682643812949945</v>
       </c>
       <c r="E98">
-        <v>0.9983886672417165</v>
+        <v>1.00815870592714</v>
       </c>
       <c r="F98">
         <v>0.9316531503880114</v>
       </c>
       <c r="G98">
-        <v>0.8901743469132578</v>
+        <v>0.8503546955774944</v>
       </c>
       <c r="H98">
-        <v>0.9731319538627651</v>
+        <v>1.012951605198529</v>
       </c>
     </row>
     <row r="99" spans="1:8">
@@ -2954,19 +2954,19 @@
         <v>0.9884762038839178</v>
       </c>
       <c r="D99">
-        <v>0.9784885352617189</v>
+        <v>0.9689003733844079</v>
       </c>
       <c r="E99">
-        <v>0.9984638725061167</v>
+        <v>1.008052034383428</v>
       </c>
       <c r="F99">
         <v>0.9332986321064581</v>
       </c>
       <c r="G99">
-        <v>0.8926233348524172</v>
+        <v>0.8535750494885378</v>
       </c>
       <c r="H99">
-        <v>0.9739739293604991</v>
+        <v>1.013022214724379</v>
       </c>
     </row>
     <row r="100" spans="1:8">
@@ -2980,19 +2980,19 @@
         <v>0.9887323918280081</v>
       </c>
       <c r="D100">
-        <v>0.9789289946090451</v>
+        <v>0.9695177332788407</v>
       </c>
       <c r="E100">
-        <v>0.998535789046971</v>
+        <v>1.007947050377175</v>
       </c>
       <c r="F100">
         <v>0.9348911172139334</v>
       </c>
       <c r="G100">
-        <v>0.894999366908254</v>
+        <v>0.8567032866148018</v>
       </c>
       <c r="H100">
-        <v>0.9747828675196127</v>
+        <v>1.013078947813065</v>
       </c>
     </row>
   </sheetData>

</xml_diff>